<commit_message>
Update schematic, library & misc; Add new datasheet & specification
</commit_message>
<xml_diff>
--- a/lib_schematic_pcb/PartList_FreePCX_v0.4.0.xlsx
+++ b/lib_schematic_pcb/PartList_FreePCX_v0.4.0.xlsx
@@ -294,7 +294,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,6 +395,30 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="9.35"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="9">
@@ -585,7 +609,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -704,9 +728,6 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -725,6 +746,33 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,40 +782,41 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1785,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,17 +1849,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="61" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
       <c r="H1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1824,16 +1873,16 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A2" s="62">
+      <c r="A2" s="57">
         <f ca="1">TODAY()</f>
-        <v>42669</v>
-      </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
+        <v>42670</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1847,32 +1896,32 @@
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="64" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="65"/>
-      <c r="G3" s="58" t="s">
+      <c r="F3" s="60"/>
+      <c r="G3" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
     </row>
     <row r="7" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
@@ -1907,17 +1956,17 @@
       <c r="I8" s="31"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1948,30 +1997,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+    <row r="11" spans="1:14" s="74" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="67">
         <v>1</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="70">
         <v>1</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="72">
         <v>136.5</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="73"/>
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -1979,7 +2028,7 @@
       <c r="C12" s="32"/>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="53"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="15"/>
@@ -2000,7 +2049,7 @@
       <c r="E13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="53" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="14">
@@ -2015,7 +2064,7 @@
       <c r="C14" s="32"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="54"/>
+      <c r="F14" s="53"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
@@ -2036,7 +2085,7 @@
       <c r="E15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="53" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="14">
@@ -2051,7 +2100,7 @@
       <c r="C16" s="32"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="54"/>
+      <c r="F16" s="53"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
@@ -2072,7 +2121,7 @@
       <c r="E17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="53" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="14">
@@ -2087,35 +2136,35 @@
       <c r="C18" s="32"/>
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="54"/>
+      <c r="F18" s="53"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="67">
         <v>5</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="70">
         <v>2</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="54" t="s">
+      <c r="F19" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="72">
         <v>14.48</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="73"/>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -2123,35 +2172,35 @@
       <c r="C20" s="32"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="54"/>
+      <c r="F20" s="53"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="67">
         <v>6</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="70">
         <v>1</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="54" t="s">
+      <c r="F21" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="72">
         <v>18.920000000000002</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="73"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -2159,35 +2208,35 @@
       <c r="C22" s="32"/>
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="54"/>
+      <c r="F22" s="53"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="67">
         <v>7</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="70">
         <v>1</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="72">
         <v>9.59</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="73"/>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -2195,35 +2244,35 @@
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="54"/>
+      <c r="F24" s="53"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="67">
         <v>8</v>
       </c>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="50">
+      <c r="D25" s="70">
         <v>1</v>
       </c>
-      <c r="E25" s="67" t="s">
+      <c r="E25" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="54" t="s">
+      <c r="F25" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="53">
+      <c r="G25" s="72">
         <v>1.88</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
@@ -2237,29 +2286,29 @@
       <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="67">
         <v>9</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="70">
         <v>1</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="72">
         <v>11.59</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="73"/>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -2273,29 +2322,29 @@
       <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="67">
         <v>10</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="47">
+      <c r="D29" s="70">
         <v>1</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="72">
         <v>17.13</v>
       </c>
-      <c r="H29" s="14"/>
-      <c r="I29" s="15"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="73"/>
     </row>
     <row r="30" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
@@ -2381,29 +2430,29 @@
       <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="A35" s="67">
         <v>13</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="70">
         <v>1</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="23" t="s">
+      <c r="F35" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="72">
         <v>7.71</v>
       </c>
-      <c r="H35" s="14"/>
-      <c r="I35" s="15"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="73"/>
     </row>
     <row r="36" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
@@ -2417,29 +2466,29 @@
       <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="A37" s="67">
         <v>14</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="70">
         <v>1</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="72">
         <v>1.67</v>
       </c>
-      <c r="H37" s="14"/>
-      <c r="I37" s="15"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="73"/>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -2453,29 +2502,29 @@
       <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="A39" s="67">
         <v>15</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="43" t="s">
+      <c r="C39" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="70">
         <v>1</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="43" t="s">
+      <c r="F39" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="72">
         <v>3.61</v>
       </c>
-      <c r="H39" s="14"/>
-      <c r="I39" s="15"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="73"/>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -2525,29 +2574,29 @@
       <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="A43" s="67">
         <v>17</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="43" t="s">
+      <c r="C43" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D43" s="70">
         <v>1</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="F43" s="43" t="s">
+      <c r="F43" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="72">
         <v>1.66</v>
       </c>
-      <c r="H43" s="14"/>
-      <c r="I43" s="15"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="73"/>
     </row>
     <row r="44" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
@@ -2561,74 +2610,74 @@
       <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="A45" s="67">
         <v>18</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="43" t="s">
+      <c r="C45" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D45" s="11">
+      <c r="D45" s="70">
         <v>1</v>
       </c>
-      <c r="E45" s="68" t="s">
+      <c r="E45" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="43" t="s">
+      <c r="F45" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="72">
         <v>12.11</v>
       </c>
-      <c r="H45" s="14"/>
-      <c r="I45" s="15"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="73"/>
     </row>
     <row r="46" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="10"/>
       <c r="C46" s="32"/>
       <c r="D46" s="11"/>
-      <c r="E46" s="68"/>
+      <c r="E46" s="55"/>
       <c r="F46" s="13"/>
       <c r="G46" s="14"/>
       <c r="H46" s="14"/>
       <c r="I46" s="15"/>
     </row>
     <row r="47" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+      <c r="A47" s="67">
         <v>19</v>
       </c>
-      <c r="B47" s="49" t="s">
+      <c r="B47" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="43" t="s">
+      <c r="C47" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="50">
+      <c r="D47" s="70">
         <v>1</v>
       </c>
-      <c r="E47" s="69" t="s">
+      <c r="E47" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="43" t="s">
+      <c r="F47" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="53">
+      <c r="G47" s="72">
         <v>7.65</v>
       </c>
-      <c r="H47" s="14"/>
-      <c r="I47" s="15"/>
+      <c r="H47" s="72"/>
+      <c r="I47" s="73"/>
     </row>
     <row r="48" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="53"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="52"/>
       <c r="H48" s="14"/>
       <c r="I48" s="15"/>
     </row>
@@ -2645,7 +2694,7 @@
       <c r="D49" s="11">
         <v>1</v>
       </c>
-      <c r="E49" s="68" t="s">
+      <c r="E49" s="55" t="s">
         <v>74</v>
       </c>
       <c r="F49" s="43" t="s">
@@ -2659,12 +2708,12 @@
     </row>
     <row r="50" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="53"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="52"/>
       <c r="H50" s="14"/>
       <c r="I50" s="15"/>
     </row>
@@ -2672,22 +2721,22 @@
       <c r="A51" s="9">
         <v>21</v>
       </c>
-      <c r="B51" s="49" t="s">
+      <c r="B51" s="48" t="s">
         <v>77</v>
       </c>
       <c r="C51" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="50">
+      <c r="D51" s="49">
         <v>1</v>
       </c>
-      <c r="E51" s="67" t="s">
+      <c r="E51" s="54" t="s">
         <v>78</v>
       </c>
       <c r="F51" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="G51" s="53">
+      <c r="G51" s="52">
         <v>1.91</v>
       </c>
       <c r="H51" s="14"/>
@@ -2695,12 +2744,12 @@
     </row>
     <row r="52" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
-      <c r="B52" s="49"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="53"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="52"/>
       <c r="H52" s="14"/>
       <c r="I52" s="15"/>
     </row>
@@ -2708,25 +2757,25 @@
       <c r="A53" s="9">
         <v>22</v>
       </c>
-      <c r="B53" s="49" t="s">
+      <c r="B53" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="49"/>
-      <c r="D53" s="50"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="53"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="49"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="52"/>
       <c r="H53" s="14"/>
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
-      <c r="B54" s="49"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="50"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="53"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="52"/>
       <c r="H54" s="14"/>
       <c r="I54" s="15"/>
     </row>
@@ -2734,25 +2783,25 @@
       <c r="A55" s="9">
         <v>23</v>
       </c>
-      <c r="B55" s="49" t="s">
+      <c r="B55" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="49"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="51"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="53"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="52"/>
       <c r="H55" s="14"/>
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="52"/>
-      <c r="G56" s="53"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="52"/>
       <c r="H56" s="14"/>
       <c r="I56" s="15"/>
     </row>
@@ -2760,25 +2809,25 @@
       <c r="A57" s="9">
         <v>24</v>
       </c>
-      <c r="B57" s="49" t="s">
+      <c r="B57" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="50"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="52"/>
-      <c r="G57" s="53"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="52"/>
       <c r="H57" s="14"/>
       <c r="I57" s="15"/>
     </row>
     <row r="58" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="50"/>
-      <c r="E58" s="51"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="53"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="52"/>
       <c r="H58" s="14"/>
       <c r="I58" s="15"/>
     </row>
@@ -2786,25 +2835,25 @@
       <c r="A59" s="9">
         <v>25</v>
       </c>
-      <c r="B59" s="49" t="s">
+      <c r="B59" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="49"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="51"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="53"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="52"/>
       <c r="H59" s="14"/>
       <c r="I59" s="15"/>
     </row>
     <row r="60" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
-      <c r="B60" s="49"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="50"/>
-      <c r="E60" s="51"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="53"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="52"/>
       <c r="H60" s="14"/>
       <c r="I60" s="15"/>
     </row>
@@ -2812,14 +2861,14 @@
       <c r="A61" s="9">
         <v>26</v>
       </c>
-      <c r="B61" s="49" t="s">
+      <c r="B61" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="C61" s="49"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="51"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="53"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="52"/>
       <c r="H61" s="14"/>
       <c r="I61" s="15"/>
     </row>
@@ -2968,30 +3017,30 @@
       <c r="I73" s="22"/>
     </row>
     <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="56" t="s">
+      <c r="A74" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="56"/>
-      <c r="C74" s="56"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56"/>
-      <c r="G74" s="56"/>
-      <c r="H74" s="56"/>
+      <c r="B74" s="64"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="64"/>
+      <c r="H74" s="64"/>
       <c r="I74" s="24">
         <f>SUMPRODUCT(ICs[Amount DDP, Kiev, Ukraine],ICs[Qty per module])</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="57" t="s">
+      <c r="A75" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="57"/>
-      <c r="C75" s="57"/>
-      <c r="D75" s="57"/>
-      <c r="E75" s="57"/>
-      <c r="F75" s="57"/>
+      <c r="B75" s="65"/>
+      <c r="C75" s="65"/>
+      <c r="D75" s="65"/>
+      <c r="E75" s="65"/>
+      <c r="F75" s="65"/>
       <c r="G75" s="26">
         <f>SUMPRODUCT(ICs[Qty per module],ICs[Disributor price, USD])</f>
         <v>288.03000000000003</v>
@@ -3000,17 +3049,17 @@
       <c r="I75" s="25"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="55" t="s">
+      <c r="A78" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B78" s="55"/>
-      <c r="C78" s="55"/>
-      <c r="D78" s="55"/>
-      <c r="E78" s="55"/>
-      <c r="F78" s="55"/>
-      <c r="G78" s="55"/>
-      <c r="H78" s="55"/>
-      <c r="I78" s="55"/>
+      <c r="B78" s="63"/>
+      <c r="C78" s="63"/>
+      <c r="D78" s="63"/>
+      <c r="E78" s="63"/>
+      <c r="F78" s="63"/>
+      <c r="G78" s="63"/>
+      <c r="H78" s="63"/>
+      <c r="I78" s="63"/>
     </row>
     <row r="79" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
@@ -3317,30 +3366,30 @@
       <c r="I104" s="22"/>
     </row>
     <row r="105" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="56" t="s">
+      <c r="A105" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B105" s="56"/>
-      <c r="C105" s="56"/>
-      <c r="D105" s="56"/>
-      <c r="E105" s="56"/>
-      <c r="F105" s="56"/>
-      <c r="G105" s="56"/>
-      <c r="H105" s="56"/>
+      <c r="B105" s="64"/>
+      <c r="C105" s="64"/>
+      <c r="D105" s="64"/>
+      <c r="E105" s="64"/>
+      <c r="F105" s="64"/>
+      <c r="G105" s="64"/>
+      <c r="H105" s="64"/>
       <c r="I105" s="24">
         <f>SUMPRODUCT(Connectors[Amount DDP, Kiev, Ukraine],Connectors[Qty per module])</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="57" t="s">
+      <c r="A106" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B106" s="57"/>
-      <c r="C106" s="57"/>
-      <c r="D106" s="57"/>
-      <c r="E106" s="57"/>
-      <c r="F106" s="57"/>
+      <c r="B106" s="65"/>
+      <c r="C106" s="65"/>
+      <c r="D106" s="65"/>
+      <c r="E106" s="65"/>
+      <c r="F106" s="65"/>
       <c r="G106" s="26">
         <f>SUMPRODUCT(Connectors[Qty per module],Connectors[Disributor price, USD])</f>
         <v>0</v>
@@ -3350,11 +3399,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C1:G2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A3:D3"/>
     <mergeCell ref="A78:I78"/>
     <mergeCell ref="A105:H105"/>
     <mergeCell ref="A106:F106"/>
@@ -3363,6 +3407,11 @@
     <mergeCell ref="A75:F75"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="A9:I9"/>
+    <mergeCell ref="C1:G2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="H80:I104 G80:G89 G91:G103">
     <cfRule type="dataBar" priority="40">
@@ -3400,7 +3449,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G92 H104">
+  <conditionalFormatting sqref="H104 G92">
     <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Update PartList, Schematic and PCB
</commit_message>
<xml_diff>
--- a/lib_schematic_pcb/PartList_FreePCX_v0.4.0.xlsx
+++ b/lib_schematic_pcb/PartList_FreePCX_v0.4.0.xlsx
@@ -294,7 +294,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +419,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -722,9 +728,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -751,39 +754,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="14" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -819,6 +789,40 @@
     <xf numFmtId="49" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1834,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1849,17 +1853,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
       <c r="H1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1873,16 +1877,16 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A2" s="57">
+      <c r="A2" s="74">
         <f ca="1">TODAY()</f>
-        <v>42670</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+        <v>42700</v>
+      </c>
+      <c r="B2" s="74"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
       <c r="H2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1896,32 +1900,32 @@
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="59" t="s">
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61" t="s">
+      <c r="F3" s="77"/>
+      <c r="G3" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
     </row>
     <row r="7" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
@@ -1956,17 +1960,17 @@
       <c r="I8" s="31"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1997,30 +2001,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="74" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="67">
+    <row r="11" spans="1:14" s="62" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="55">
         <v>1</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="70">
+      <c r="D11" s="58">
         <v>1</v>
       </c>
-      <c r="E11" s="71" t="s">
+      <c r="E11" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="69" t="s">
+      <c r="F11" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="72">
+      <c r="G11" s="60">
         <v>136.5</v>
       </c>
-      <c r="H11" s="72"/>
-      <c r="I11" s="73"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="61"/>
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -2028,7 +2032,7 @@
       <c r="C12" s="32"/>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="53"/>
+      <c r="F12" s="52"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="15"/>
@@ -2049,7 +2053,7 @@
       <c r="E13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="53" t="s">
+      <c r="F13" s="52" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="14">
@@ -2064,35 +2068,35 @@
       <c r="C14" s="32"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="53"/>
+      <c r="F14" s="52"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
     </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+    <row r="15" spans="1:14" s="78" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="55">
         <v>3</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="58">
         <v>2</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="53" t="s">
+      <c r="F15" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="60">
         <v>1.76</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="61"/>
     </row>
     <row r="16" spans="1:14" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
@@ -2100,35 +2104,35 @@
       <c r="C16" s="32"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="53"/>
+      <c r="F16" s="52"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="55">
         <v>4</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="58">
         <v>1</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="53" t="s">
+      <c r="F17" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="60">
         <v>0.4</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="61"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -2136,35 +2140,35 @@
       <c r="C18" s="32"/>
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="53"/>
+      <c r="F18" s="52"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="67">
+      <c r="A19" s="55">
         <v>5</v>
       </c>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="70">
+      <c r="D19" s="58">
         <v>2</v>
       </c>
-      <c r="E19" s="71" t="s">
+      <c r="E19" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="75" t="s">
+      <c r="F19" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="72">
+      <c r="G19" s="60">
         <v>14.48</v>
       </c>
-      <c r="H19" s="72"/>
-      <c r="I19" s="73"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="61"/>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -2172,35 +2176,35 @@
       <c r="C20" s="32"/>
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="53"/>
+      <c r="F20" s="52"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="67">
+      <c r="A21" s="55">
         <v>6</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="58">
         <v>1</v>
       </c>
-      <c r="E21" s="71" t="s">
+      <c r="E21" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="75" t="s">
+      <c r="F21" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="72">
+      <c r="G21" s="60">
         <v>18.920000000000002</v>
       </c>
-      <c r="H21" s="72"/>
-      <c r="I21" s="73"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="61"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
@@ -2208,35 +2212,35 @@
       <c r="C22" s="32"/>
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="53"/>
+      <c r="F22" s="52"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="67">
+      <c r="A23" s="55">
         <v>7</v>
       </c>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="69" t="s">
+      <c r="C23" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="70">
+      <c r="D23" s="58">
         <v>1</v>
       </c>
-      <c r="E23" s="71" t="s">
+      <c r="E23" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="75" t="s">
+      <c r="F23" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="72">
+      <c r="G23" s="60">
         <v>9.59</v>
       </c>
-      <c r="H23" s="72"/>
-      <c r="I23" s="73"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="61"/>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
@@ -2244,41 +2248,41 @@
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="53"/>
+      <c r="F24" s="52"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="67">
+      <c r="A25" s="55">
         <v>8</v>
       </c>
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="69" t="s">
+      <c r="C25" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="70">
+      <c r="D25" s="58">
         <v>1</v>
       </c>
-      <c r="E25" s="71" t="s">
+      <c r="E25" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="75" t="s">
+      <c r="F25" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="72">
+      <c r="G25" s="60">
         <v>1.88</v>
       </c>
-      <c r="H25" s="72"/>
-      <c r="I25" s="73"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="61"/>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
-      <c r="D26" s="47"/>
+      <c r="D26" s="46"/>
       <c r="E26" s="12"/>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
@@ -2286,35 +2290,35 @@
       <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="67">
+      <c r="A27" s="55">
         <v>9</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="76" t="s">
+      <c r="C27" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="70">
+      <c r="D27" s="58">
         <v>1</v>
       </c>
-      <c r="E27" s="71" t="s">
+      <c r="E27" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="69" t="s">
+      <c r="F27" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="72">
+      <c r="G27" s="60">
         <v>11.59</v>
       </c>
-      <c r="H27" s="72"/>
-      <c r="I27" s="73"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="61"/>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
-      <c r="D28" s="47"/>
+      <c r="D28" s="46"/>
       <c r="E28" s="12"/>
       <c r="F28" s="13"/>
       <c r="G28" s="14"/>
@@ -2322,35 +2326,35 @@
       <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="67">
+      <c r="A29" s="55">
         <v>10</v>
       </c>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="69" t="s">
+      <c r="C29" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="70">
+      <c r="D29" s="58">
         <v>1</v>
       </c>
-      <c r="E29" s="71" t="s">
+      <c r="E29" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="69" t="s">
+      <c r="F29" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="72">
+      <c r="G29" s="60">
         <v>17.13</v>
       </c>
-      <c r="H29" s="72"/>
-      <c r="I29" s="73"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="61"/>
     </row>
     <row r="30" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="45"/>
       <c r="C30" s="45"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="46"/>
       <c r="E30" s="12"/>
       <c r="F30" s="13"/>
       <c r="G30" s="14"/>
@@ -2358,29 +2362,29 @@
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="55">
         <v>11</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="47">
+      <c r="D31" s="58">
         <v>1</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="23" t="s">
+      <c r="F31" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="60">
         <v>2.76</v>
       </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="61"/>
     </row>
     <row r="32" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -2394,29 +2398,29 @@
       <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="55">
         <v>12</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="58">
         <v>1</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="23" t="s">
+      <c r="F33" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="60">
         <v>4.51</v>
       </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="15"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="61"/>
     </row>
     <row r="34" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
@@ -2430,29 +2434,29 @@
       <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A35" s="67">
+      <c r="A35" s="55">
         <v>13</v>
       </c>
-      <c r="B35" s="68" t="s">
+      <c r="B35" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="69" t="s">
+      <c r="C35" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="70">
+      <c r="D35" s="58">
         <v>1</v>
       </c>
-      <c r="E35" s="71" t="s">
+      <c r="E35" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="69" t="s">
+      <c r="F35" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="72">
+      <c r="G35" s="60">
         <v>7.71</v>
       </c>
-      <c r="H35" s="72"/>
-      <c r="I35" s="73"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="61"/>
     </row>
     <row r="36" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
@@ -2466,29 +2470,29 @@
       <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="67">
+      <c r="A37" s="55">
         <v>14</v>
       </c>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="69" t="s">
+      <c r="C37" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="70">
+      <c r="D37" s="58">
         <v>1</v>
       </c>
-      <c r="E37" s="71" t="s">
+      <c r="E37" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="69" t="s">
+      <c r="F37" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G37" s="72">
+      <c r="G37" s="60">
         <v>1.67</v>
       </c>
-      <c r="H37" s="72"/>
-      <c r="I37" s="73"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="61"/>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
@@ -2502,29 +2506,29 @@
       <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="67">
+      <c r="A39" s="55">
         <v>15</v>
       </c>
-      <c r="B39" s="68" t="s">
+      <c r="B39" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="77" t="s">
+      <c r="C39" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="70">
+      <c r="D39" s="58">
         <v>1</v>
       </c>
-      <c r="E39" s="71" t="s">
+      <c r="E39" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="77" t="s">
+      <c r="F39" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="G39" s="72">
+      <c r="G39" s="60">
         <v>3.61</v>
       </c>
-      <c r="H39" s="72"/>
-      <c r="I39" s="73"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="61"/>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
@@ -2574,29 +2578,29 @@
       <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="67">
+      <c r="A43" s="55">
         <v>17</v>
       </c>
-      <c r="B43" s="68" t="s">
+      <c r="B43" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="77" t="s">
+      <c r="C43" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="70">
+      <c r="D43" s="58">
         <v>1</v>
       </c>
-      <c r="E43" s="71" t="s">
+      <c r="E43" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="F43" s="77" t="s">
+      <c r="F43" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="72">
+      <c r="G43" s="60">
         <v>1.66</v>
       </c>
-      <c r="H43" s="72"/>
-      <c r="I43" s="73"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="61"/>
     </row>
     <row r="44" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
@@ -2610,74 +2614,74 @@
       <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="67">
+      <c r="A45" s="55">
         <v>18</v>
       </c>
-      <c r="B45" s="68" t="s">
+      <c r="B45" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="77" t="s">
+      <c r="C45" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="D45" s="70">
+      <c r="D45" s="58">
         <v>1</v>
       </c>
-      <c r="E45" s="78" t="s">
+      <c r="E45" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="77" t="s">
+      <c r="F45" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="72">
+      <c r="G45" s="60">
         <v>12.11</v>
       </c>
-      <c r="H45" s="72"/>
-      <c r="I45" s="73"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="61"/>
     </row>
     <row r="46" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="10"/>
       <c r="C46" s="32"/>
       <c r="D46" s="11"/>
-      <c r="E46" s="55"/>
+      <c r="E46" s="54"/>
       <c r="F46" s="13"/>
       <c r="G46" s="14"/>
       <c r="H46" s="14"/>
       <c r="I46" s="15"/>
     </row>
     <row r="47" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="67">
+      <c r="A47" s="55">
         <v>19</v>
       </c>
-      <c r="B47" s="68" t="s">
+      <c r="B47" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="77" t="s">
+      <c r="C47" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="70">
+      <c r="D47" s="58">
         <v>1</v>
       </c>
-      <c r="E47" s="78" t="s">
+      <c r="E47" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="77" t="s">
+      <c r="F47" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="72">
+      <c r="G47" s="60">
         <v>7.65</v>
       </c>
-      <c r="H47" s="72"/>
-      <c r="I47" s="73"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="61"/>
     </row>
     <row r="48" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="52"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="51"/>
       <c r="H48" s="14"/>
       <c r="I48" s="15"/>
     </row>
@@ -2694,7 +2698,7 @@
       <c r="D49" s="11">
         <v>1</v>
       </c>
-      <c r="E49" s="55" t="s">
+      <c r="E49" s="54" t="s">
         <v>74</v>
       </c>
       <c r="F49" s="43" t="s">
@@ -2708,12 +2712,12 @@
     </row>
     <row r="50" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="48"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="52"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="51"/>
       <c r="H50" s="14"/>
       <c r="I50" s="15"/>
     </row>
@@ -2721,22 +2725,22 @@
       <c r="A51" s="9">
         <v>21</v>
       </c>
-      <c r="B51" s="48" t="s">
+      <c r="B51" s="47" t="s">
         <v>77</v>
       </c>
       <c r="C51" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="49">
+      <c r="D51" s="48">
         <v>1</v>
       </c>
-      <c r="E51" s="54" t="s">
+      <c r="E51" s="53" t="s">
         <v>78</v>
       </c>
       <c r="F51" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="G51" s="52">
+      <c r="G51" s="51">
         <v>1.91</v>
       </c>
       <c r="H51" s="14"/>
@@ -2744,12 +2748,12 @@
     </row>
     <row r="52" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
-      <c r="B52" s="48"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="49"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="52"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="51"/>
       <c r="H52" s="14"/>
       <c r="I52" s="15"/>
     </row>
@@ -2757,25 +2761,25 @@
       <c r="A53" s="9">
         <v>22</v>
       </c>
-      <c r="B53" s="48" t="s">
+      <c r="B53" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="48"/>
-      <c r="D53" s="49"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="52"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="51"/>
       <c r="H53" s="14"/>
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="52"/>
+      <c r="B54" s="47"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="51"/>
       <c r="H54" s="14"/>
       <c r="I54" s="15"/>
     </row>
@@ -2783,25 +2787,25 @@
       <c r="A55" s="9">
         <v>23</v>
       </c>
-      <c r="B55" s="48" t="s">
+      <c r="B55" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="48"/>
-      <c r="D55" s="49"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="51"/>
-      <c r="G55" s="52"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="51"/>
       <c r="H55" s="14"/>
       <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="51"/>
-      <c r="G56" s="52"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="51"/>
       <c r="H56" s="14"/>
       <c r="I56" s="15"/>
     </row>
@@ -2809,25 +2813,25 @@
       <c r="A57" s="9">
         <v>24</v>
       </c>
-      <c r="B57" s="48" t="s">
+      <c r="B57" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="51"/>
-      <c r="G57" s="52"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="51"/>
       <c r="H57" s="14"/>
       <c r="I57" s="15"/>
     </row>
     <row r="58" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
-      <c r="B58" s="48"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="51"/>
-      <c r="G58" s="52"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="51"/>
       <c r="H58" s="14"/>
       <c r="I58" s="15"/>
     </row>
@@ -2835,25 +2839,25 @@
       <c r="A59" s="9">
         <v>25</v>
       </c>
-      <c r="B59" s="48" t="s">
+      <c r="B59" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="48"/>
-      <c r="D59" s="49"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="51"/>
-      <c r="G59" s="52"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="51"/>
       <c r="H59" s="14"/>
       <c r="I59" s="15"/>
     </row>
     <row r="60" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="49"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="51"/>
-      <c r="G60" s="52"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="48"/>
+      <c r="E60" s="49"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="51"/>
       <c r="H60" s="14"/>
       <c r="I60" s="15"/>
     </row>
@@ -2861,14 +2865,14 @@
       <c r="A61" s="9">
         <v>26</v>
       </c>
-      <c r="B61" s="48" t="s">
+      <c r="B61" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C61" s="48"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="51"/>
-      <c r="G61" s="52"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="51"/>
       <c r="H61" s="14"/>
       <c r="I61" s="15"/>
     </row>
@@ -3017,30 +3021,30 @@
       <c r="I73" s="22"/>
     </row>
     <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="64" t="s">
+      <c r="A74" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="64"/>
-      <c r="C74" s="64"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="64"/>
-      <c r="F74" s="64"/>
-      <c r="G74" s="64"/>
-      <c r="H74" s="64"/>
+      <c r="B74" s="68"/>
+      <c r="C74" s="68"/>
+      <c r="D74" s="68"/>
+      <c r="E74" s="68"/>
+      <c r="F74" s="68"/>
+      <c r="G74" s="68"/>
+      <c r="H74" s="68"/>
       <c r="I74" s="24">
         <f>SUMPRODUCT(ICs[Amount DDP, Kiev, Ukraine],ICs[Qty per module])</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="65" t="s">
+      <c r="A75" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="65"/>
-      <c r="C75" s="65"/>
-      <c r="D75" s="65"/>
-      <c r="E75" s="65"/>
-      <c r="F75" s="65"/>
+      <c r="B75" s="69"/>
+      <c r="C75" s="69"/>
+      <c r="D75" s="69"/>
+      <c r="E75" s="69"/>
+      <c r="F75" s="69"/>
       <c r="G75" s="26">
         <f>SUMPRODUCT(ICs[Qty per module],ICs[Disributor price, USD])</f>
         <v>288.03000000000003</v>
@@ -3049,17 +3053,17 @@
       <c r="I75" s="25"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="63" t="s">
+      <c r="A78" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B78" s="63"/>
-      <c r="C78" s="63"/>
-      <c r="D78" s="63"/>
-      <c r="E78" s="63"/>
-      <c r="F78" s="63"/>
-      <c r="G78" s="63"/>
-      <c r="H78" s="63"/>
-      <c r="I78" s="63"/>
+      <c r="B78" s="67"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="67"/>
+      <c r="E78" s="67"/>
+      <c r="F78" s="67"/>
+      <c r="G78" s="67"/>
+      <c r="H78" s="67"/>
+      <c r="I78" s="67"/>
     </row>
     <row r="79" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
@@ -3366,30 +3370,30 @@
       <c r="I104" s="22"/>
     </row>
     <row r="105" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="64" t="s">
+      <c r="A105" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="B105" s="64"/>
-      <c r="C105" s="64"/>
-      <c r="D105" s="64"/>
-      <c r="E105" s="64"/>
-      <c r="F105" s="64"/>
-      <c r="G105" s="64"/>
-      <c r="H105" s="64"/>
+      <c r="B105" s="68"/>
+      <c r="C105" s="68"/>
+      <c r="D105" s="68"/>
+      <c r="E105" s="68"/>
+      <c r="F105" s="68"/>
+      <c r="G105" s="68"/>
+      <c r="H105" s="68"/>
       <c r="I105" s="24">
         <f>SUMPRODUCT(Connectors[Amount DDP, Kiev, Ukraine],Connectors[Qty per module])</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="65" t="s">
+      <c r="A106" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B106" s="65"/>
-      <c r="C106" s="65"/>
-      <c r="D106" s="65"/>
-      <c r="E106" s="65"/>
-      <c r="F106" s="65"/>
+      <c r="B106" s="69"/>
+      <c r="C106" s="69"/>
+      <c r="D106" s="69"/>
+      <c r="E106" s="69"/>
+      <c r="F106" s="69"/>
       <c r="G106" s="26">
         <f>SUMPRODUCT(Connectors[Qty per module],Connectors[Disributor price, USD])</f>
         <v>0</v>
@@ -3399,6 +3403,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C1:G2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A3:D3"/>
     <mergeCell ref="A78:I78"/>
     <mergeCell ref="A105:H105"/>
     <mergeCell ref="A106:F106"/>
@@ -3407,11 +3416,6 @@
     <mergeCell ref="A75:F75"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="A9:I9"/>
-    <mergeCell ref="C1:G2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="H80:I104 G80:G89 G91:G103">
     <cfRule type="dataBar" priority="40">
@@ -3449,7 +3453,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H104 G92">
+  <conditionalFormatting sqref="G92 H104">
     <cfRule type="dataBar" priority="30">
       <dataBar>
         <cfvo type="min"/>

</xml_diff>